<commit_message>
added noise correction function to signal processing
</commit_message>
<xml_diff>
--- a/Hydrophones/Noise_Correction/matching_tau_results/noise_correction_results.xlsx
+++ b/Hydrophones/Noise_Correction/matching_tau_results/noise_correction_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Noise_Correction\matching_tau_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F1755F-16DC-4482-A57A-66AAEE430A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF009ED-2A79-4D68-80C7-73445EA209B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9055,8 +9055,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.167001312335958"/>
-                  <c:y val="4.0546293979977437E-2"/>
+                  <c:x val="0.11807802323534589"/>
+                  <c:y val="0.25683774982124219"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -9228,132 +9228,132 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2023'!$AJ$3:$AJ$43</c:f>
+              <c:f>'2023'!$AK$3:$AK$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>1.9808443158627718</c:v>
+                  <c:v>1.6023306164916791</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2848181540971852</c:v>
+                  <c:v>1.8926401087257059</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9078328190789398</c:v>
+                  <c:v>1.577603180434239</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9235207880521508</c:v>
+                  <c:v>1.597388805942314</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9174864955048601</c:v>
+                  <c:v>1.6112210905025457</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4394365654148733</c:v>
+                  <c:v>1.2122713639881819</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5903776368248552</c:v>
+                  <c:v>1.3482955315054186</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5417389589585446</c:v>
+                  <c:v>1.3157050589480173</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4765327098839185</c:v>
+                  <c:v>1.2909197425904744</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.5336706220263248</c:v>
+                  <c:v>1.3090641585820353</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6161974848639291</c:v>
+                  <c:v>1.383903921758401</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6150878323822884</c:v>
+                  <c:v>1.3887865720771682</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.7044302959241602</c:v>
+                  <c:v>1.4934617519613649</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5641806970005112</c:v>
+                  <c:v>1.3827064936056632</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.5503118669298432</c:v>
+                  <c:v>1.3107124009498248</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.123350367217987</c:v>
+                  <c:v>1.8707195415844995</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1458173813193011</c:v>
+                  <c:v>1.8776761238817394</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3272955276167679</c:v>
+                  <c:v>2.026910506833465</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1809157705505924</c:v>
+                  <c:v>1.888208101080491</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1346539341112565</c:v>
+                  <c:v>1.9104443325974683</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.1659468106384274</c:v>
+                  <c:v>2.6064926314559962</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.7579554849312959</c:v>
+                  <c:v>2.2878878617036391</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.1735140761531322</c:v>
+                  <c:v>2.6833012668439662</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.1607496451743375</c:v>
+                  <c:v>2.6653962014377943</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.0727075446661334</c:v>
+                  <c:v>2.549979683940669</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.1251915217198092</c:v>
+                  <c:v>2.4612516748957671</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.0068867226904823</c:v>
+                  <c:v>2.4063567540574682</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.734687239845969</c:v>
+                  <c:v>2.1818978925511177</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.8060076562383629</c:v>
+                  <c:v>2.2568865874345612</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.5217211102089689</c:v>
+                  <c:v>2.0354709857785531</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.5357886486673351</c:v>
+                  <c:v>2.7951368943409269</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.1919039500240127</c:v>
+                  <c:v>2.6244411915732213</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.2472699349087217</c:v>
+                  <c:v>2.6251161008006578</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.8217302436069573</c:v>
+                  <c:v>2.2603454807980481</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.9548946560621983</c:v>
+                  <c:v>2.3265732500183569</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.9157053990067849</c:v>
+                  <c:v>2.3299771857227998</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.0220291666132009</c:v>
+                  <c:v>2.4018397612574764</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.4269831735356644</c:v>
+                  <c:v>1.9741671576379574</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.5415184977662006</c:v>
+                  <c:v>2.0320099467288526</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.5078116373487878</c:v>
+                  <c:v>2.0349829161848532</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.5992611993727723</c:v>
+                  <c:v>2.0977470987795193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9417,8 +9417,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.18730720773031542"/>
-                  <c:y val="0.2246607822683514"/>
+                  <c:x val="0.10763535772264539"/>
+                  <c:y val="0.35903628086966483"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -30374,8 +30374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN80"/>
   <sheetViews>
-    <sheetView topLeftCell="P13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH51" sqref="AH51"/>
+    <sheetView topLeftCell="T27" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AE54" sqref="AE54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36752,8 +36752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38F4079-A6EE-4070-A855-6EDAE9ED1E0C}">
   <dimension ref="A1:AO88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AF54" sqref="AF54"/>
+    <sheetView tabSelected="1" topLeftCell="U33" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="AH41" sqref="AH41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40160,15 +40160,15 @@
         <v>2.3865552327512338</v>
       </c>
       <c r="AK45" s="9">
-        <f t="shared" ref="AK45:AO45" si="7">AVERAGE(AK3:AK43)</f>
+        <f>AVERAGE(AK3:AK43)</f>
         <v>1.9738592177556802</v>
       </c>
       <c r="AL45" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AK45:AO45" si="7">AVERAGE(AL3:AL43)</f>
         <v>3.7085609496792515</v>
       </c>
       <c r="AM45" s="9">
-        <f t="shared" si="7"/>
+        <f>AVERAGE(AM3:AM43)</f>
         <v>1.9690905584264888</v>
       </c>
       <c r="AN45" s="7">

</xml_diff>